<commit_message>
Reading for release v0.12.0
</commit_message>
<xml_diff>
--- a/tests/siteinvestigation/insitutests/data/spt_example_layering.xlsx
+++ b/tests/siteinvestigation/insitutests/data/spt_example_layering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/SourceTree.tmp/ProFound/groundhog/tests/siteinvestigation/insitutests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bstuyts/Documents/Code/ProFound/groundhog/tests/siteinvestigation/insitutests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFAB365-FCD7-5A47-9264-E0EED39FEC20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3638CE0-FA00-5148-BA52-A21A8147DF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{43740A81-3D27-F54D-9F09-31244D1F9D12}"/>
+    <workbookView xWindow="16920" yWindow="760" windowWidth="16680" windowHeight="20400" xr2:uid="{43740A81-3D27-F54D-9F09-31244D1F9D12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Depth from [ft]</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>SILTSTONE</t>
+  </si>
+  <si>
+    <t>Granular</t>
   </si>
 </sst>
 </file>
@@ -116,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -262,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -404,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2F065E-DD47-CF45-A796-0A2E37FD4B2F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,7 +429,7 @@
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +442,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -453,8 +459,11 @@
       <c r="D2">
         <v>16</v>
       </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.4</v>
       </c>
@@ -467,8 +476,11 @@
       <c r="D3">
         <v>19</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -481,8 +493,11 @@
       <c r="D4">
         <v>17</v>
       </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -495,8 +510,11 @@
       <c r="D5">
         <v>18.5</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>29.5</v>
       </c>
@@ -508,6 +526,9 @@
       </c>
       <c r="D6">
         <v>21</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>